<commit_message>
updated list, including main group 52 for alcohols
</commit_message>
<xml_diff>
--- a/AIOMFAC_Documents/List_of_AIOMFAC_Maingroups_and_Subgroups.xlsx
+++ b/AIOMFAC_Documents/List_of_AIOMFAC_Maingroups_and_Subgroups.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andiz\Dropbox\AIOMFAC_WebInterface\AIOMFAC-web_3.00\Additional_Files_For_GitHub_online\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andiz\Documents\Work_McGill\Models_Code\AIOMFAC-Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC72FC7-246B-4EC8-A056-046B005AE342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50E1BF6-3F55-4546-968E-5F859B9CEEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="239">
   <si>
     <t>hydroxyl</t>
   </si>
@@ -224,9 +235,6 @@
   </si>
   <si>
     <t>(C=C)</t>
-  </si>
-  <si>
-    <t>CHn[OH]</t>
   </si>
   <si>
     <t>CHn[alc]</t>
@@ -750,6 +758,18 @@
   </si>
   <si>
     <t>as part of bicarbonate-containing mixtures</t>
+  </si>
+  <si>
+    <t>CH2[OH]</t>
+  </si>
+  <si>
+    <t>we use main group 52 for CH[OH] and C[OH] as they refer to CHn bonded to secondary or tertiary hydroxyl/alcohol</t>
+  </si>
+  <si>
+    <t>we use main group 68 for CH2 bonded to primary hydroxyl/alcohol</t>
+  </si>
+  <si>
+    <t>CH[OH]</t>
   </si>
 </sst>
 </file>
@@ -843,7 +863,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -899,6 +919,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1148,11 +1174,10 @@
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1192,7 +1217,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1224,6 +1248,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" xfId="4" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="10" borderId="12" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" xfId="4" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1234,13 +1266,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1280,9 +1313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1320,9 +1353,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1355,26 +1388,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1407,26 +1423,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1603,36 +1602,36 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:UA101"/>
+  <dimension ref="A1:UA102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
-    <col min="8" max="8" width="150.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="3.08984375" customWidth="1"/>
+    <col min="6" max="6" width="24.453125" customWidth="1"/>
+    <col min="7" max="7" width="29.6328125" customWidth="1"/>
+    <col min="8" max="8" width="150.90625" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:547" s="18" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+    <row r="1" spans="1:547" s="17" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
       <c r="BN1"/>
       <c r="BO1"/>
       <c r="BP1"/>
@@ -2116,9 +2115,9 @@
       <c r="TZ1"/>
       <c r="UA1"/>
     </row>
-    <row r="2" spans="1:547" s="17" customFormat="1">
-      <c r="A2" s="17" t="s">
-        <v>194</v>
+    <row r="2" spans="1:547" s="16" customFormat="1">
+      <c r="A2" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="BN2"/>
       <c r="BO2"/>
@@ -2603,9 +2602,9 @@
       <c r="TZ2"/>
       <c r="UA2"/>
     </row>
-    <row r="3" spans="1:547" s="17" customFormat="1">
-      <c r="A3" s="25" t="s">
-        <v>199</v>
+    <row r="3" spans="1:547" s="16" customFormat="1">
+      <c r="A3" t="s">
+        <v>198</v>
       </c>
       <c r="BN3"/>
       <c r="BO3"/>
@@ -3090,7 +3089,7 @@
       <c r="TZ3"/>
       <c r="UA3"/>
     </row>
-    <row r="4" spans="1:547" s="17" customFormat="1" ht="15" thickBot="1">
+    <row r="4" spans="1:547" s="16" customFormat="1" ht="15" thickBot="1">
       <c r="BN4"/>
       <c r="BO4"/>
       <c r="BP4"/>
@@ -3575,315 +3574,315 @@
       <c r="UA4"/>
     </row>
     <row r="5" spans="1:547" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A5" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="A5" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="45" t="s">
-        <v>198</v>
-      </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="20" t="s">
+      <c r="E5" s="42"/>
+      <c r="F5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:547" ht="21.75" customHeight="1" thickBot="1">
+      <c r="A6" s="56" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="59"/>
+    </row>
+    <row r="7" spans="1:547">
+      <c r="A7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="33">
+        <v>1</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="11" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:547" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A6" s="51" t="s">
-        <v>193</v>
-      </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="54"/>
-    </row>
-    <row r="7" spans="1:547">
-      <c r="A7" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="G7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="12"/>
+    </row>
+    <row r="8" spans="1:547">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="34">
+        <v>2</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:547">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="34">
+        <v>3</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:547">
+      <c r="A10" s="9"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="34">
+        <v>4</v>
+      </c>
+      <c r="E10" s="28"/>
+      <c r="F10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:547">
+      <c r="A11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2</v>
+      </c>
+      <c r="D11" s="35">
+        <v>5</v>
+      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:547">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="35">
+        <v>6</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:547">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="35">
+        <v>7</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:547">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="35">
+        <v>8</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:547">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="35">
+        <v>70</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:547">
+      <c r="A16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="24">
+        <v>3</v>
+      </c>
+      <c r="D16" s="34">
         <v>9</v>
       </c>
-      <c r="C7" s="26">
-        <v>1</v>
-      </c>
-      <c r="D7" s="35">
-        <v>1</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:547">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="36">
-        <v>2</v>
-      </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:547">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="36">
-        <v>3</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:547">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="36">
+      <c r="E16" s="28"/>
+      <c r="F16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:547">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="34">
+        <v>10</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:547" s="2" customFormat="1">
+      <c r="A18" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="26">
         <v>4</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:547">
-      <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="27">
-        <v>2</v>
-      </c>
-      <c r="D11" s="37">
-        <v>5</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:547">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="37">
-        <v>6</v>
-      </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:547">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="37">
-        <v>7</v>
-      </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:547">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="37">
-        <v>8</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:547">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="37">
-        <v>70</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:547">
-      <c r="A16" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="26">
-        <v>3</v>
-      </c>
-      <c r="D16" s="36">
-        <v>9</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:547">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="36">
-        <v>10</v>
-      </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="11" t="s">
+      <c r="D18" s="36">
+        <v>11</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:547" s="2" customFormat="1">
-      <c r="A18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="28">
-        <v>4</v>
-      </c>
-      <c r="D18" s="38">
-        <v>11</v>
-      </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="15" t="s">
+      <c r="G18" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>191</v>
+      <c r="H18" s="13" t="s">
+        <v>190</v>
       </c>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
-      <c r="AK18" s="3"/>
-      <c r="AL18" s="3"/>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
-      <c r="AP18" s="3"/>
-      <c r="AQ18" s="3"/>
-      <c r="AR18" s="3"/>
-      <c r="AS18" s="3"/>
-      <c r="AT18" s="3"/>
-      <c r="AU18" s="3"/>
-      <c r="AV18" s="3"/>
-      <c r="AW18" s="3"/>
-      <c r="AX18" s="3"/>
-      <c r="AY18" s="3"/>
-      <c r="AZ18" s="3"/>
-      <c r="BA18" s="3"/>
-      <c r="BB18" s="3"/>
-      <c r="BC18" s="3"/>
-      <c r="BD18" s="3"/>
-      <c r="BE18" s="3"/>
-      <c r="BF18" s="3"/>
-      <c r="BG18" s="3"/>
-      <c r="BH18" s="3"/>
-      <c r="BI18" s="3"/>
-      <c r="BJ18" s="3"/>
-      <c r="BK18" s="3"/>
-      <c r="BL18" s="3"/>
-      <c r="BM18" s="3"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+      <c r="BE18"/>
+      <c r="BF18"/>
+      <c r="BG18"/>
+      <c r="BH18"/>
+      <c r="BI18"/>
+      <c r="BJ18"/>
+      <c r="BK18"/>
+      <c r="BL18"/>
+      <c r="BM18"/>
       <c r="BN18"/>
       <c r="BO18"/>
       <c r="BP18"/>
@@ -4368,77 +4367,77 @@
       <c r="UA18"/>
     </row>
     <row r="19" spans="1:547" s="2" customFormat="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="38">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="36">
         <v>12</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="15" t="s">
+      <c r="E19" s="30"/>
+      <c r="F19" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="H19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" s="13"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
-      <c r="AL19" s="3"/>
-      <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
-      <c r="AP19" s="3"/>
-      <c r="AQ19" s="3"/>
-      <c r="AR19" s="3"/>
-      <c r="AS19" s="3"/>
-      <c r="AT19" s="3"/>
-      <c r="AU19" s="3"/>
-      <c r="AV19" s="3"/>
-      <c r="AW19" s="3"/>
-      <c r="AX19" s="3"/>
-      <c r="AY19" s="3"/>
-      <c r="AZ19" s="3"/>
-      <c r="BA19" s="3"/>
-      <c r="BB19" s="3"/>
-      <c r="BC19" s="3"/>
-      <c r="BD19" s="3"/>
-      <c r="BE19" s="3"/>
-      <c r="BF19" s="3"/>
-      <c r="BG19" s="3"/>
-      <c r="BH19" s="3"/>
-      <c r="BI19" s="3"/>
-      <c r="BJ19" s="3"/>
-      <c r="BK19" s="3"/>
-      <c r="BL19" s="3"/>
-      <c r="BM19" s="3"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+      <c r="BE19"/>
+      <c r="BF19"/>
+      <c r="BG19"/>
+      <c r="BH19"/>
+      <c r="BI19"/>
+      <c r="BJ19"/>
+      <c r="BK19"/>
+      <c r="BL19"/>
+      <c r="BM19"/>
       <c r="BN19"/>
       <c r="BO19"/>
       <c r="BP19"/>
@@ -4923,77 +4922,77 @@
       <c r="UA19"/>
     </row>
     <row r="20" spans="1:547" s="2" customFormat="1">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="38">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="36">
         <v>13</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="H20" s="14"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" s="13"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="3"/>
-      <c r="AJ20" s="3"/>
-      <c r="AK20" s="3"/>
-      <c r="AL20" s="3"/>
-      <c r="AM20" s="3"/>
-      <c r="AN20" s="3"/>
-      <c r="AO20" s="3"/>
-      <c r="AP20" s="3"/>
-      <c r="AQ20" s="3"/>
-      <c r="AR20" s="3"/>
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
-      <c r="AW20" s="3"/>
-      <c r="AX20" s="3"/>
-      <c r="AY20" s="3"/>
-      <c r="AZ20" s="3"/>
-      <c r="BA20" s="3"/>
-      <c r="BB20" s="3"/>
-      <c r="BC20" s="3"/>
-      <c r="BD20" s="3"/>
-      <c r="BE20" s="3"/>
-      <c r="BF20" s="3"/>
-      <c r="BG20" s="3"/>
-      <c r="BH20" s="3"/>
-      <c r="BI20" s="3"/>
-      <c r="BJ20" s="3"/>
-      <c r="BK20" s="3"/>
-      <c r="BL20" s="3"/>
-      <c r="BM20" s="3"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20"/>
+      <c r="BF20"/>
+      <c r="BG20"/>
+      <c r="BH20"/>
+      <c r="BI20"/>
+      <c r="BJ20"/>
+      <c r="BK20"/>
+      <c r="BL20"/>
+      <c r="BM20"/>
       <c r="BN20"/>
       <c r="BO20"/>
       <c r="BP20"/>
@@ -5478,1884 +5477,1902 @@
       <c r="UA20"/>
     </row>
     <row r="21" spans="1:547">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="25">
         <v>69</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="35">
         <v>153</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="7" t="s">
+      <c r="E21" s="29"/>
+      <c r="F21" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="H21" s="7"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:547">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="24">
         <v>8</v>
       </c>
-      <c r="D22" s="36">
+      <c r="D22" s="34">
         <v>17</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="11" t="s">
+      <c r="E22" s="28"/>
+      <c r="F22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="11"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:547">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="24">
         <v>9</v>
       </c>
-      <c r="D23" s="36">
+      <c r="D23" s="34">
         <v>18</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="28"/>
+      <c r="F23" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:547">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="34">
+        <v>19</v>
+      </c>
+      <c r="E24" s="28"/>
+      <c r="F24" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" spans="1:547">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="36">
-        <v>19</v>
-      </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="H24" s="10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:547">
+      <c r="A25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="25">
+        <v>10</v>
+      </c>
+      <c r="D25" s="35">
+        <v>20</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="G25" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:547">
+      <c r="A26" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="24">
+        <v>11</v>
+      </c>
+      <c r="D26" s="34">
+        <v>21</v>
+      </c>
+      <c r="E26" s="28"/>
+      <c r="F26" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:547">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="34">
+        <v>22</v>
+      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:547">
+      <c r="A28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="25">
+        <v>13</v>
+      </c>
+      <c r="D28" s="35">
+        <v>24</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:547">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="35">
+        <v>25</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:547">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="35">
+        <v>26</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:547">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="25"/>
+      <c r="D31" s="35">
+        <v>27</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:547">
+      <c r="A32" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>231</v>
+      </c>
+      <c r="D32" s="34">
+        <v>137</v>
+      </c>
+      <c r="E32" s="28"/>
+      <c r="F32" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="37">
+        <v>43</v>
+      </c>
+      <c r="E33" s="28"/>
+      <c r="F33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="25">
+        <v>66</v>
+      </c>
+      <c r="D34" s="35">
+        <v>141</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="35">
+        <v>142</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="35">
+        <v>143</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="35">
+        <v>144</v>
+      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" ht="29">
+      <c r="A38" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="24">
+        <v>67</v>
+      </c>
+      <c r="D38" s="34">
+        <v>145</v>
+      </c>
+      <c r="E38" s="28"/>
+      <c r="F38" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="34">
+        <v>146</v>
+      </c>
+      <c r="E39" s="28"/>
+      <c r="F39" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="34">
+        <v>147</v>
+      </c>
+      <c r="E40" s="28"/>
+      <c r="F40" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="9"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="34">
+        <v>148</v>
+      </c>
+      <c r="E41" s="28"/>
+      <c r="F41" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" ht="29">
+      <c r="A42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="25">
+        <v>68</v>
+      </c>
+      <c r="D42" s="35">
+        <v>149</v>
+      </c>
+      <c r="E42" s="29"/>
+      <c r="F42" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="35">
+        <v>150</v>
+      </c>
+      <c r="E43" s="29"/>
+      <c r="F43" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="5"/>
+      <c r="B45" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" s="55">
+        <v>52</v>
+      </c>
+      <c r="D45" s="35">
+        <v>151</v>
+      </c>
+      <c r="E45" s="29"/>
+      <c r="F45" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="8"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="35">
+        <v>152</v>
+      </c>
+      <c r="E46" s="29"/>
+      <c r="F46" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="8"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="26">
+        <v>70</v>
+      </c>
+      <c r="D48" s="38">
+        <v>154</v>
+      </c>
+      <c r="E48" s="30"/>
+      <c r="F48" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="G48" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="8"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="24">
+        <v>71</v>
+      </c>
+      <c r="D50" s="34">
+        <v>155</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="12"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="34">
+        <v>156</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="12"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="34">
+        <v>157</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="H52" s="10"/>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="25">
+        <v>72</v>
+      </c>
+      <c r="D53" s="35">
+        <v>158</v>
+      </c>
+      <c r="E53" s="29"/>
+      <c r="F53" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="H53" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="8"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="35">
+        <v>159</v>
+      </c>
+      <c r="E54" s="29"/>
+      <c r="F54" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="8"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="25"/>
+      <c r="D55" s="35">
+        <v>160</v>
+      </c>
+      <c r="E55" s="29"/>
+      <c r="F55" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="A56" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="24">
+        <v>73</v>
+      </c>
+      <c r="D56" s="34">
+        <v>161</v>
+      </c>
+      <c r="E56" s="28"/>
+      <c r="F56" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C57" s="27">
+        <v>74</v>
+      </c>
+      <c r="D57" s="39">
+        <v>162</v>
+      </c>
+      <c r="E57" s="32"/>
+      <c r="F57" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="A58" s="22"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="39">
+        <v>163</v>
+      </c>
+      <c r="E58" s="32"/>
+      <c r="F58" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="G58" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="A59" s="22"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="27"/>
+      <c r="D59" s="39">
+        <v>164</v>
+      </c>
+      <c r="E59" s="32"/>
+      <c r="F59" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="22"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="39">
+        <v>165</v>
+      </c>
+      <c r="E60" s="32"/>
+      <c r="F60" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="22"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="39">
+        <v>166</v>
+      </c>
+      <c r="E61" s="32"/>
+      <c r="F61" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="22"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="39">
+        <v>167</v>
+      </c>
+      <c r="E62" s="32"/>
+      <c r="F62" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="G62" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="A63" s="22"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="27"/>
+      <c r="D63" s="39">
+        <v>168</v>
+      </c>
+      <c r="E63" s="32"/>
+      <c r="F63" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="H63" s="15"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="22"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="27"/>
+      <c r="D64" s="39">
+        <v>169</v>
+      </c>
+      <c r="E64" s="32"/>
+      <c r="F64" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="H64" s="15"/>
+    </row>
+    <row r="65" spans="1:547">
+      <c r="A65" s="22"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="39">
+        <v>170</v>
+      </c>
+      <c r="E65" s="32"/>
+      <c r="F65" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="H65" s="15"/>
+    </row>
+    <row r="66" spans="1:547">
+      <c r="A66" s="22"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="39">
+        <v>171</v>
+      </c>
+      <c r="E66" s="32"/>
+      <c r="F66" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:547">
+      <c r="A67" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67" s="24">
+        <v>75</v>
+      </c>
+      <c r="D67" s="34">
+        <v>172</v>
+      </c>
+      <c r="E67" s="28"/>
+      <c r="F67" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:547" s="51" customFormat="1">
+      <c r="A68" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>213</v>
+      </c>
+      <c r="C68" s="47">
+        <v>76</v>
+      </c>
+      <c r="D68" s="48">
+        <v>173</v>
+      </c>
+      <c r="E68" s="49"/>
+      <c r="F68" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="G68" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="H68" s="46" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="69" spans="1:547">
+      <c r="A69" s="8"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="35"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="1:547">
+      <c r="A70" s="8"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="25"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:547" s="3" customFormat="1" ht="15" thickBot="1">
+      <c r="A71" s="63"/>
+      <c r="B71" s="63"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="63"/>
+      <c r="F71" s="63"/>
+      <c r="G71" s="63"/>
+      <c r="H71" s="63"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71"/>
+      <c r="Y71"/>
+      <c r="Z71"/>
+      <c r="AA71"/>
+      <c r="AB71"/>
+      <c r="AC71"/>
+      <c r="AD71"/>
+      <c r="AE71"/>
+      <c r="AF71"/>
+      <c r="AG71"/>
+      <c r="AH71"/>
+      <c r="AI71"/>
+      <c r="AJ71"/>
+      <c r="AK71"/>
+      <c r="AL71"/>
+      <c r="AM71"/>
+      <c r="AN71"/>
+      <c r="AO71"/>
+      <c r="AP71"/>
+      <c r="AQ71"/>
+      <c r="AR71"/>
+      <c r="AS71"/>
+      <c r="AT71"/>
+      <c r="AU71"/>
+      <c r="AV71"/>
+      <c r="AW71"/>
+      <c r="AX71"/>
+      <c r="AY71"/>
+      <c r="AZ71"/>
+      <c r="BA71"/>
+      <c r="BB71"/>
+      <c r="BC71"/>
+      <c r="BD71"/>
+      <c r="BE71"/>
+      <c r="BF71"/>
+      <c r="BG71"/>
+      <c r="BH71"/>
+      <c r="BI71"/>
+      <c r="BJ71"/>
+      <c r="BK71"/>
+      <c r="BL71"/>
+      <c r="BM71"/>
+      <c r="BN71"/>
+      <c r="BO71"/>
+      <c r="BP71"/>
+      <c r="BQ71"/>
+      <c r="BR71"/>
+      <c r="BS71"/>
+      <c r="BT71"/>
+      <c r="BU71"/>
+      <c r="BV71"/>
+      <c r="BW71"/>
+      <c r="BX71"/>
+      <c r="BY71"/>
+      <c r="BZ71"/>
+      <c r="CA71"/>
+      <c r="CB71"/>
+      <c r="CC71"/>
+      <c r="CD71"/>
+      <c r="CE71"/>
+      <c r="CF71"/>
+      <c r="CG71"/>
+      <c r="CH71"/>
+      <c r="CI71"/>
+      <c r="CJ71"/>
+      <c r="CK71"/>
+      <c r="CL71"/>
+      <c r="CM71"/>
+      <c r="CN71"/>
+      <c r="CO71"/>
+      <c r="CP71"/>
+      <c r="CQ71"/>
+      <c r="CR71"/>
+      <c r="CS71"/>
+      <c r="CT71"/>
+      <c r="CU71"/>
+      <c r="CV71"/>
+      <c r="CW71"/>
+      <c r="CX71"/>
+      <c r="CY71"/>
+      <c r="CZ71"/>
+      <c r="DA71"/>
+      <c r="DB71"/>
+      <c r="DC71"/>
+      <c r="DD71"/>
+      <c r="DE71"/>
+      <c r="DF71"/>
+      <c r="DG71"/>
+      <c r="DH71"/>
+      <c r="DI71"/>
+      <c r="DJ71"/>
+      <c r="DK71"/>
+      <c r="DL71"/>
+      <c r="DM71"/>
+      <c r="DN71"/>
+      <c r="DO71"/>
+      <c r="DP71"/>
+      <c r="DQ71"/>
+      <c r="DR71"/>
+      <c r="DS71"/>
+      <c r="DT71"/>
+      <c r="DU71"/>
+      <c r="DV71"/>
+      <c r="DW71"/>
+      <c r="DX71"/>
+      <c r="DY71"/>
+      <c r="DZ71"/>
+      <c r="EA71"/>
+      <c r="EB71"/>
+      <c r="EC71"/>
+      <c r="ED71"/>
+      <c r="EE71"/>
+      <c r="EF71"/>
+      <c r="EG71"/>
+      <c r="EH71"/>
+      <c r="EI71"/>
+      <c r="EJ71"/>
+      <c r="EK71"/>
+      <c r="EL71"/>
+      <c r="EM71"/>
+      <c r="EN71"/>
+      <c r="EO71"/>
+      <c r="EP71"/>
+      <c r="EQ71"/>
+      <c r="ER71"/>
+      <c r="ES71"/>
+      <c r="ET71"/>
+      <c r="EU71"/>
+      <c r="EV71"/>
+      <c r="EW71"/>
+      <c r="EX71"/>
+      <c r="EY71"/>
+      <c r="EZ71"/>
+      <c r="FA71"/>
+      <c r="FB71"/>
+      <c r="FC71"/>
+      <c r="FD71"/>
+      <c r="FE71"/>
+      <c r="FF71"/>
+      <c r="FG71"/>
+      <c r="FH71"/>
+      <c r="FI71"/>
+      <c r="FJ71"/>
+      <c r="FK71"/>
+      <c r="FL71"/>
+      <c r="FM71"/>
+      <c r="FN71"/>
+      <c r="FO71"/>
+      <c r="FP71"/>
+      <c r="FQ71"/>
+      <c r="FR71"/>
+      <c r="FS71"/>
+      <c r="FT71"/>
+      <c r="FU71"/>
+      <c r="FV71"/>
+      <c r="FW71"/>
+      <c r="FX71"/>
+      <c r="FY71"/>
+      <c r="FZ71"/>
+      <c r="GA71"/>
+      <c r="GB71"/>
+      <c r="GC71"/>
+      <c r="GD71"/>
+      <c r="GE71"/>
+      <c r="GF71"/>
+      <c r="GG71"/>
+      <c r="GH71"/>
+      <c r="GI71"/>
+      <c r="GJ71"/>
+      <c r="GK71"/>
+      <c r="GL71"/>
+      <c r="GM71"/>
+      <c r="GN71"/>
+      <c r="GO71"/>
+      <c r="GP71"/>
+      <c r="GQ71"/>
+      <c r="GR71"/>
+      <c r="GS71"/>
+      <c r="GT71"/>
+      <c r="GU71"/>
+      <c r="GV71"/>
+      <c r="GW71"/>
+      <c r="GX71"/>
+      <c r="GY71"/>
+      <c r="GZ71"/>
+      <c r="HA71"/>
+      <c r="HB71"/>
+      <c r="HC71"/>
+      <c r="HD71"/>
+      <c r="HE71"/>
+      <c r="HF71"/>
+      <c r="HG71"/>
+      <c r="HH71"/>
+      <c r="HI71"/>
+      <c r="HJ71"/>
+      <c r="HK71"/>
+      <c r="HL71"/>
+      <c r="HM71"/>
+      <c r="HN71"/>
+      <c r="HO71"/>
+      <c r="HP71"/>
+      <c r="HQ71"/>
+      <c r="HR71"/>
+      <c r="HS71"/>
+      <c r="HT71"/>
+      <c r="HU71"/>
+      <c r="HV71"/>
+      <c r="HW71"/>
+      <c r="HX71"/>
+      <c r="HY71"/>
+      <c r="HZ71"/>
+      <c r="IA71"/>
+      <c r="IB71"/>
+      <c r="IC71"/>
+      <c r="ID71"/>
+      <c r="IE71"/>
+      <c r="IF71"/>
+      <c r="IG71"/>
+      <c r="IH71"/>
+      <c r="II71"/>
+      <c r="IJ71"/>
+      <c r="IK71"/>
+      <c r="IL71"/>
+      <c r="IM71"/>
+      <c r="IN71"/>
+      <c r="IO71"/>
+      <c r="IP71"/>
+      <c r="IQ71"/>
+      <c r="IR71"/>
+      <c r="IS71"/>
+      <c r="IT71"/>
+      <c r="IU71"/>
+      <c r="IV71"/>
+      <c r="IW71"/>
+      <c r="IX71"/>
+      <c r="IY71"/>
+      <c r="IZ71"/>
+      <c r="JA71"/>
+      <c r="JB71"/>
+      <c r="JC71"/>
+      <c r="JD71"/>
+      <c r="JE71"/>
+      <c r="JF71"/>
+      <c r="JG71"/>
+      <c r="JH71"/>
+      <c r="JI71"/>
+      <c r="JJ71"/>
+      <c r="JK71"/>
+      <c r="JL71"/>
+      <c r="JM71"/>
+      <c r="JN71"/>
+      <c r="JO71"/>
+      <c r="JP71"/>
+      <c r="JQ71"/>
+      <c r="JR71"/>
+      <c r="JS71"/>
+      <c r="JT71"/>
+      <c r="JU71"/>
+      <c r="JV71"/>
+      <c r="JW71"/>
+      <c r="JX71"/>
+      <c r="JY71"/>
+      <c r="JZ71"/>
+      <c r="KA71"/>
+      <c r="KB71"/>
+      <c r="KC71"/>
+      <c r="KD71"/>
+      <c r="KE71"/>
+      <c r="KF71"/>
+      <c r="KG71"/>
+      <c r="KH71"/>
+      <c r="KI71"/>
+      <c r="KJ71"/>
+      <c r="KK71"/>
+      <c r="KL71"/>
+      <c r="KM71"/>
+      <c r="KN71"/>
+      <c r="KO71"/>
+      <c r="KP71"/>
+      <c r="KQ71"/>
+      <c r="KR71"/>
+      <c r="KS71"/>
+      <c r="KT71"/>
+      <c r="KU71"/>
+      <c r="KV71"/>
+      <c r="KW71"/>
+      <c r="KX71"/>
+      <c r="KY71"/>
+      <c r="KZ71"/>
+      <c r="LA71"/>
+      <c r="LB71"/>
+      <c r="LC71"/>
+      <c r="LD71"/>
+      <c r="LE71"/>
+      <c r="LF71"/>
+      <c r="LG71"/>
+      <c r="LH71"/>
+      <c r="LI71"/>
+      <c r="LJ71"/>
+      <c r="LK71"/>
+      <c r="LL71"/>
+      <c r="LM71"/>
+      <c r="LN71"/>
+      <c r="LO71"/>
+      <c r="LP71"/>
+      <c r="LQ71"/>
+      <c r="LR71"/>
+      <c r="LS71"/>
+      <c r="LT71"/>
+      <c r="LU71"/>
+      <c r="LV71"/>
+      <c r="LW71"/>
+      <c r="LX71"/>
+      <c r="LY71"/>
+      <c r="LZ71"/>
+      <c r="MA71"/>
+      <c r="MB71"/>
+      <c r="MC71"/>
+      <c r="MD71"/>
+      <c r="ME71"/>
+      <c r="MF71"/>
+      <c r="MG71"/>
+      <c r="MH71"/>
+      <c r="MI71"/>
+      <c r="MJ71"/>
+      <c r="MK71"/>
+      <c r="ML71"/>
+      <c r="MM71"/>
+      <c r="MN71"/>
+      <c r="MO71"/>
+      <c r="MP71"/>
+      <c r="MQ71"/>
+      <c r="MR71"/>
+      <c r="MS71"/>
+      <c r="MT71"/>
+      <c r="MU71"/>
+      <c r="MV71"/>
+      <c r="MW71"/>
+      <c r="MX71"/>
+      <c r="MY71"/>
+      <c r="MZ71"/>
+      <c r="NA71"/>
+      <c r="NB71"/>
+      <c r="NC71"/>
+      <c r="ND71"/>
+      <c r="NE71"/>
+      <c r="NF71"/>
+      <c r="NG71"/>
+      <c r="NH71"/>
+      <c r="NI71"/>
+      <c r="NJ71"/>
+      <c r="NK71"/>
+      <c r="NL71"/>
+      <c r="NM71"/>
+      <c r="NN71"/>
+      <c r="NO71"/>
+      <c r="NP71"/>
+      <c r="NQ71"/>
+      <c r="NR71"/>
+      <c r="NS71"/>
+      <c r="NT71"/>
+      <c r="NU71"/>
+      <c r="NV71"/>
+      <c r="NW71"/>
+      <c r="NX71"/>
+      <c r="NY71"/>
+      <c r="NZ71"/>
+      <c r="OA71"/>
+      <c r="OB71"/>
+      <c r="OC71"/>
+      <c r="OD71"/>
+      <c r="OE71"/>
+      <c r="OF71"/>
+      <c r="OG71"/>
+      <c r="OH71"/>
+      <c r="OI71"/>
+      <c r="OJ71"/>
+      <c r="OK71"/>
+      <c r="OL71"/>
+      <c r="OM71"/>
+      <c r="ON71"/>
+      <c r="OO71"/>
+      <c r="OP71"/>
+      <c r="OQ71"/>
+      <c r="OR71"/>
+      <c r="OS71"/>
+      <c r="OT71"/>
+      <c r="OU71"/>
+      <c r="OV71"/>
+      <c r="OW71"/>
+      <c r="OX71"/>
+      <c r="OY71"/>
+      <c r="OZ71"/>
+      <c r="PA71"/>
+      <c r="PB71"/>
+      <c r="PC71"/>
+      <c r="PD71"/>
+      <c r="PE71"/>
+      <c r="PF71"/>
+      <c r="PG71"/>
+      <c r="PH71"/>
+      <c r="PI71"/>
+      <c r="PJ71"/>
+      <c r="PK71"/>
+      <c r="PL71"/>
+      <c r="PM71"/>
+      <c r="PN71"/>
+      <c r="PO71"/>
+      <c r="PP71"/>
+      <c r="PQ71"/>
+      <c r="PR71"/>
+      <c r="PS71"/>
+      <c r="PT71"/>
+      <c r="PU71"/>
+      <c r="PV71"/>
+      <c r="PW71"/>
+      <c r="PX71"/>
+      <c r="PY71"/>
+      <c r="PZ71"/>
+      <c r="QA71"/>
+      <c r="QB71"/>
+      <c r="QC71"/>
+      <c r="QD71"/>
+      <c r="QE71"/>
+      <c r="QF71"/>
+      <c r="QG71"/>
+      <c r="QH71"/>
+      <c r="QI71"/>
+      <c r="QJ71"/>
+      <c r="QK71"/>
+      <c r="QL71"/>
+      <c r="QM71"/>
+      <c r="QN71"/>
+      <c r="QO71"/>
+      <c r="QP71"/>
+      <c r="QQ71"/>
+      <c r="QR71"/>
+      <c r="QS71"/>
+      <c r="QT71"/>
+      <c r="QU71"/>
+      <c r="QV71"/>
+      <c r="QW71"/>
+      <c r="QX71"/>
+      <c r="QY71"/>
+      <c r="QZ71"/>
+      <c r="RA71"/>
+      <c r="RB71"/>
+      <c r="RC71"/>
+      <c r="RD71"/>
+      <c r="RE71"/>
+      <c r="RF71"/>
+      <c r="RG71"/>
+      <c r="RH71"/>
+      <c r="RI71"/>
+      <c r="RJ71"/>
+      <c r="RK71"/>
+      <c r="RL71"/>
+      <c r="RM71"/>
+      <c r="RN71"/>
+      <c r="RO71"/>
+      <c r="RP71"/>
+      <c r="RQ71"/>
+      <c r="RR71"/>
+      <c r="RS71"/>
+      <c r="RT71"/>
+      <c r="RU71"/>
+      <c r="RV71"/>
+      <c r="RW71"/>
+      <c r="RX71"/>
+      <c r="RY71"/>
+      <c r="RZ71"/>
+      <c r="SA71"/>
+      <c r="SB71"/>
+      <c r="SC71"/>
+      <c r="SD71"/>
+      <c r="SE71"/>
+      <c r="SF71"/>
+      <c r="SG71"/>
+      <c r="SH71"/>
+      <c r="SI71"/>
+      <c r="SJ71"/>
+      <c r="SK71"/>
+      <c r="SL71"/>
+      <c r="SM71"/>
+      <c r="SN71"/>
+      <c r="SO71"/>
+      <c r="SP71"/>
+      <c r="SQ71"/>
+      <c r="SR71"/>
+      <c r="SS71"/>
+      <c r="ST71"/>
+      <c r="SU71"/>
+      <c r="SV71"/>
+      <c r="SW71"/>
+      <c r="SX71"/>
+      <c r="SY71"/>
+      <c r="SZ71"/>
+      <c r="TA71"/>
+      <c r="TB71"/>
+      <c r="TC71"/>
+      <c r="TD71"/>
+      <c r="TE71"/>
+      <c r="TF71"/>
+      <c r="TG71"/>
+      <c r="TH71"/>
+      <c r="TI71"/>
+      <c r="TJ71"/>
+      <c r="TK71"/>
+      <c r="TL71"/>
+      <c r="TM71"/>
+      <c r="TN71"/>
+      <c r="TO71"/>
+      <c r="TP71"/>
+      <c r="TQ71"/>
+      <c r="TR71"/>
+      <c r="TS71"/>
+      <c r="TT71"/>
+      <c r="TU71"/>
+      <c r="TV71"/>
+      <c r="TW71"/>
+      <c r="TX71"/>
+      <c r="TY71"/>
+      <c r="TZ71"/>
+      <c r="UA71"/>
+    </row>
+    <row r="72" spans="1:547" ht="19" thickTop="1">
+      <c r="A72" s="60" t="s">
+        <v>191</v>
+      </c>
+      <c r="B72" s="61"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="61"/>
+      <c r="E72" s="61"/>
+      <c r="F72" s="61"/>
+      <c r="G72" s="61"/>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="1:547">
+      <c r="A73" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="25"/>
+      <c r="D73" s="40">
+        <v>205</v>
+      </c>
+      <c r="E73" s="29"/>
+      <c r="F73" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:547">
+      <c r="A74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="25"/>
+      <c r="D74" s="40">
+        <v>201</v>
+      </c>
+      <c r="E74" s="29"/>
+      <c r="F74" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:547">
+      <c r="A75" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="40">
+        <v>202</v>
+      </c>
+      <c r="E75" s="29"/>
+      <c r="F75" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="76" spans="1:547">
+      <c r="A76" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="40">
+        <v>203</v>
+      </c>
+      <c r="E76" s="29"/>
+      <c r="F76" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H76" s="6"/>
+    </row>
+    <row r="77" spans="1:547">
+      <c r="A77" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="40">
+        <v>204</v>
+      </c>
+      <c r="E77" s="29"/>
+      <c r="F77" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H77" s="6"/>
+    </row>
+    <row r="78" spans="1:547">
+      <c r="A78" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="40">
+        <v>223</v>
+      </c>
+      <c r="E78" s="29"/>
+      <c r="F78" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H78" s="6"/>
+    </row>
+    <row r="79" spans="1:547">
+      <c r="A79" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="40">
+        <v>221</v>
+      </c>
+      <c r="E79" s="29"/>
+      <c r="F79" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H79" s="6"/>
+    </row>
+    <row r="80" spans="1:547">
+      <c r="A80" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="40">
+        <v>242</v>
+      </c>
+      <c r="E80" s="29"/>
+      <c r="F80" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="25"/>
+      <c r="D81" s="40">
+        <v>243</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H81" s="6"/>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="40">
+        <v>244</v>
+      </c>
+      <c r="E82" s="29"/>
+      <c r="F82" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="A83" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="25"/>
+      <c r="D83" s="40">
+        <v>245</v>
+      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="1:8">
+      <c r="A84" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="25"/>
+      <c r="D84" s="40">
+        <v>246</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="1:8">
+      <c r="A85" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="40">
+        <v>247</v>
+      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="25"/>
+      <c r="D86" s="40">
+        <v>248</v>
+      </c>
+      <c r="E86" s="29"/>
+      <c r="F86" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" s="8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="25" spans="1:547">
-      <c r="A25" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="27">
-        <v>10</v>
-      </c>
-      <c r="D25" s="37">
-        <v>20</v>
-      </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H25" s="7"/>
-    </row>
-    <row r="26" spans="1:547">
-      <c r="A26" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="26">
-        <v>11</v>
-      </c>
-      <c r="D26" s="36">
-        <v>21</v>
-      </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:547">
-      <c r="A27" s="10"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="36">
-        <v>22</v>
-      </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" spans="1:547">
-      <c r="A28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="27">
-        <v>13</v>
-      </c>
-      <c r="D28" s="37">
-        <v>24</v>
-      </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:547">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="37">
-        <v>25</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:547">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="37">
-        <v>26</v>
-      </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:547">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="37">
-        <v>27</v>
-      </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H31" s="7"/>
-    </row>
-    <row r="32" spans="1:547">
-      <c r="A32" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>232</v>
-      </c>
-      <c r="D32" s="36">
-        <v>137</v>
-      </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="11" t="s">
+      <c r="B87" s="6"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="40">
+        <v>249</v>
+      </c>
+      <c r="E87" s="29"/>
+      <c r="F87" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G87" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="53" t="s">
+        <v>206</v>
+      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="40">
+        <v>250</v>
+      </c>
+      <c r="E88" s="29"/>
+      <c r="F88" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" s="54" t="s">
+        <v>223</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="25"/>
+      <c r="D89" s="40">
+        <v>251</v>
+      </c>
+      <c r="E89" s="29"/>
+      <c r="F89" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H89" s="8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="39">
-        <v>43</v>
-      </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="27">
-        <v>66</v>
-      </c>
-      <c r="D34" s="37">
-        <v>141</v>
-      </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="37">
-        <v>142</v>
-      </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="37">
-        <v>143</v>
-      </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="37">
-        <v>144</v>
-      </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H37" s="7"/>
-    </row>
-    <row r="38" spans="1:8" ht="28.8">
-      <c r="A38" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="26">
-        <v>67</v>
-      </c>
-      <c r="D38" s="36">
-        <v>145</v>
-      </c>
-      <c r="E38" s="30"/>
-      <c r="F38" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="H38" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="10"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="36">
-        <v>146</v>
-      </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="36">
-        <v>147</v>
-      </c>
-      <c r="E40" s="30"/>
-      <c r="F40" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="10"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="36">
-        <v>148</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="H41" s="11"/>
-    </row>
-    <row r="42" spans="1:8" ht="28.8">
-      <c r="A42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" s="27">
-        <v>68</v>
-      </c>
-      <c r="D42" s="37">
-        <v>149</v>
-      </c>
-      <c r="E42" s="31"/>
-      <c r="F42" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="37">
-        <v>150</v>
-      </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G43" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="6"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="37">
-        <v>151</v>
-      </c>
-      <c r="E44" s="31"/>
-      <c r="F44" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G44" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="9"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="37">
-        <v>152</v>
-      </c>
-      <c r="E45" s="31"/>
-      <c r="F45" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="9"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="37"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="C47" s="28">
-        <v>70</v>
-      </c>
-      <c r="D47" s="40">
-        <v>154</v>
-      </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="G47" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="9"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="37"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="26">
-        <v>71</v>
-      </c>
-      <c r="D49" s="36">
-        <v>155</v>
-      </c>
-      <c r="E49" s="30"/>
-      <c r="F49" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="13"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="36">
-        <v>156</v>
-      </c>
-      <c r="E50" s="30"/>
-      <c r="F50" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H50" s="11"/>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="13"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="36">
-        <v>157</v>
-      </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H51" s="11"/>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C52" s="27">
-        <v>72</v>
-      </c>
-      <c r="D52" s="37">
-        <v>158</v>
-      </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="G52" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="9"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="37">
-        <v>159</v>
-      </c>
-      <c r="E53" s="31"/>
-      <c r="F53" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="9"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="37">
-        <v>160</v>
-      </c>
-      <c r="E54" s="31"/>
-      <c r="F54" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G54" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C55" s="26">
-        <v>73</v>
-      </c>
-      <c r="D55" s="36">
-        <v>161</v>
-      </c>
-      <c r="E55" s="30"/>
-      <c r="F55" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G55" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="B56" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C56" s="29">
-        <v>74</v>
-      </c>
-      <c r="D56" s="41">
-        <v>162</v>
-      </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="G56" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="H56" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="23"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="41">
-        <v>163</v>
-      </c>
-      <c r="E57" s="34"/>
-      <c r="F57" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="G57" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" s="16"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="23"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="41">
-        <v>164</v>
-      </c>
-      <c r="E58" s="34"/>
-      <c r="F58" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G58" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="H58" s="16"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="23"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="41">
-        <v>165</v>
-      </c>
-      <c r="E59" s="34"/>
-      <c r="F59" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="23"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="41">
-        <v>166</v>
-      </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="G60" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="23"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="41">
-        <v>167</v>
-      </c>
-      <c r="E61" s="34"/>
-      <c r="F61" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="G61" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="H61" s="16"/>
-    </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="23"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="41">
-        <v>168</v>
-      </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="G62" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="H62" s="16"/>
-    </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="23"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="41">
-        <v>169</v>
-      </c>
-      <c r="E63" s="34"/>
-      <c r="F63" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="G63" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="23"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="41">
-        <v>170</v>
-      </c>
-      <c r="E64" s="34"/>
-      <c r="F64" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="G64" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="1:547">
-      <c r="A65" s="23"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="41">
-        <v>171</v>
-      </c>
-      <c r="E65" s="34"/>
-      <c r="F65" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="G65" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:547">
-      <c r="A66" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="C66" s="26">
-        <v>75</v>
-      </c>
-      <c r="D66" s="36">
-        <v>172</v>
-      </c>
-      <c r="E66" s="30"/>
-      <c r="F66" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="H66" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="67" spans="1:547" s="47" customFormat="1">
-      <c r="A67" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C67" s="26">
-        <v>76</v>
-      </c>
-      <c r="D67" s="36">
-        <v>173</v>
-      </c>
-      <c r="E67" s="30"/>
-      <c r="F67" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="G67" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="68" spans="1:547">
-      <c r="A68" s="9"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:547">
-      <c r="A69" s="9"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:547" s="4" customFormat="1" ht="15" thickBot="1">
-      <c r="A70" s="58"/>
-      <c r="B70" s="58"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70"/>
-      <c r="J70"/>
-      <c r="K70"/>
-      <c r="L70"/>
-      <c r="M70"/>
-      <c r="N70"/>
-      <c r="O70"/>
-      <c r="P70"/>
-      <c r="Q70"/>
-      <c r="R70"/>
-      <c r="S70"/>
-      <c r="T70"/>
-      <c r="U70"/>
-      <c r="V70"/>
-      <c r="W70"/>
-      <c r="X70"/>
-      <c r="Y70"/>
-      <c r="Z70"/>
-      <c r="AA70"/>
-      <c r="AB70"/>
-      <c r="AC70"/>
-      <c r="AD70"/>
-      <c r="AE70"/>
-      <c r="AF70"/>
-      <c r="AG70"/>
-      <c r="AH70"/>
-      <c r="AI70"/>
-      <c r="AJ70"/>
-      <c r="AK70"/>
-      <c r="AL70"/>
-      <c r="AM70"/>
-      <c r="AN70"/>
-      <c r="AO70"/>
-      <c r="AP70"/>
-      <c r="AQ70"/>
-      <c r="AR70"/>
-      <c r="AS70"/>
-      <c r="AT70"/>
-      <c r="AU70"/>
-      <c r="AV70"/>
-      <c r="AW70"/>
-      <c r="AX70"/>
-      <c r="AY70"/>
-      <c r="AZ70"/>
-      <c r="BA70"/>
-      <c r="BB70"/>
-      <c r="BC70"/>
-      <c r="BD70"/>
-      <c r="BE70"/>
-      <c r="BF70"/>
-      <c r="BG70"/>
-      <c r="BH70"/>
-      <c r="BI70"/>
-      <c r="BJ70"/>
-      <c r="BK70"/>
-      <c r="BL70"/>
-      <c r="BM70"/>
-      <c r="BN70"/>
-      <c r="BO70"/>
-      <c r="BP70"/>
-      <c r="BQ70"/>
-      <c r="BR70"/>
-      <c r="BS70"/>
-      <c r="BT70"/>
-      <c r="BU70"/>
-      <c r="BV70"/>
-      <c r="BW70"/>
-      <c r="BX70"/>
-      <c r="BY70"/>
-      <c r="BZ70"/>
-      <c r="CA70"/>
-      <c r="CB70"/>
-      <c r="CC70"/>
-      <c r="CD70"/>
-      <c r="CE70"/>
-      <c r="CF70"/>
-      <c r="CG70"/>
-      <c r="CH70"/>
-      <c r="CI70"/>
-      <c r="CJ70"/>
-      <c r="CK70"/>
-      <c r="CL70"/>
-      <c r="CM70"/>
-      <c r="CN70"/>
-      <c r="CO70"/>
-      <c r="CP70"/>
-      <c r="CQ70"/>
-      <c r="CR70"/>
-      <c r="CS70"/>
-      <c r="CT70"/>
-      <c r="CU70"/>
-      <c r="CV70"/>
-      <c r="CW70"/>
-      <c r="CX70"/>
-      <c r="CY70"/>
-      <c r="CZ70"/>
-      <c r="DA70"/>
-      <c r="DB70"/>
-      <c r="DC70"/>
-      <c r="DD70"/>
-      <c r="DE70"/>
-      <c r="DF70"/>
-      <c r="DG70"/>
-      <c r="DH70"/>
-      <c r="DI70"/>
-      <c r="DJ70"/>
-      <c r="DK70"/>
-      <c r="DL70"/>
-      <c r="DM70"/>
-      <c r="DN70"/>
-      <c r="DO70"/>
-      <c r="DP70"/>
-      <c r="DQ70"/>
-      <c r="DR70"/>
-      <c r="DS70"/>
-      <c r="DT70"/>
-      <c r="DU70"/>
-      <c r="DV70"/>
-      <c r="DW70"/>
-      <c r="DX70"/>
-      <c r="DY70"/>
-      <c r="DZ70"/>
-      <c r="EA70"/>
-      <c r="EB70"/>
-      <c r="EC70"/>
-      <c r="ED70"/>
-      <c r="EE70"/>
-      <c r="EF70"/>
-      <c r="EG70"/>
-      <c r="EH70"/>
-      <c r="EI70"/>
-      <c r="EJ70"/>
-      <c r="EK70"/>
-      <c r="EL70"/>
-      <c r="EM70"/>
-      <c r="EN70"/>
-      <c r="EO70"/>
-      <c r="EP70"/>
-      <c r="EQ70"/>
-      <c r="ER70"/>
-      <c r="ES70"/>
-      <c r="ET70"/>
-      <c r="EU70"/>
-      <c r="EV70"/>
-      <c r="EW70"/>
-      <c r="EX70"/>
-      <c r="EY70"/>
-      <c r="EZ70"/>
-      <c r="FA70"/>
-      <c r="FB70"/>
-      <c r="FC70"/>
-      <c r="FD70"/>
-      <c r="FE70"/>
-      <c r="FF70"/>
-      <c r="FG70"/>
-      <c r="FH70"/>
-      <c r="FI70"/>
-      <c r="FJ70"/>
-      <c r="FK70"/>
-      <c r="FL70"/>
-      <c r="FM70"/>
-      <c r="FN70"/>
-      <c r="FO70"/>
-      <c r="FP70"/>
-      <c r="FQ70"/>
-      <c r="FR70"/>
-      <c r="FS70"/>
-      <c r="FT70"/>
-      <c r="FU70"/>
-      <c r="FV70"/>
-      <c r="FW70"/>
-      <c r="FX70"/>
-      <c r="FY70"/>
-      <c r="FZ70"/>
-      <c r="GA70"/>
-      <c r="GB70"/>
-      <c r="GC70"/>
-      <c r="GD70"/>
-      <c r="GE70"/>
-      <c r="GF70"/>
-      <c r="GG70"/>
-      <c r="GH70"/>
-      <c r="GI70"/>
-      <c r="GJ70"/>
-      <c r="GK70"/>
-      <c r="GL70"/>
-      <c r="GM70"/>
-      <c r="GN70"/>
-      <c r="GO70"/>
-      <c r="GP70"/>
-      <c r="GQ70"/>
-      <c r="GR70"/>
-      <c r="GS70"/>
-      <c r="GT70"/>
-      <c r="GU70"/>
-      <c r="GV70"/>
-      <c r="GW70"/>
-      <c r="GX70"/>
-      <c r="GY70"/>
-      <c r="GZ70"/>
-      <c r="HA70"/>
-      <c r="HB70"/>
-      <c r="HC70"/>
-      <c r="HD70"/>
-      <c r="HE70"/>
-      <c r="HF70"/>
-      <c r="HG70"/>
-      <c r="HH70"/>
-      <c r="HI70"/>
-      <c r="HJ70"/>
-      <c r="HK70"/>
-      <c r="HL70"/>
-      <c r="HM70"/>
-      <c r="HN70"/>
-      <c r="HO70"/>
-      <c r="HP70"/>
-      <c r="HQ70"/>
-      <c r="HR70"/>
-      <c r="HS70"/>
-      <c r="HT70"/>
-      <c r="HU70"/>
-      <c r="HV70"/>
-      <c r="HW70"/>
-      <c r="HX70"/>
-      <c r="HY70"/>
-      <c r="HZ70"/>
-      <c r="IA70"/>
-      <c r="IB70"/>
-      <c r="IC70"/>
-      <c r="ID70"/>
-      <c r="IE70"/>
-      <c r="IF70"/>
-      <c r="IG70"/>
-      <c r="IH70"/>
-      <c r="II70"/>
-      <c r="IJ70"/>
-      <c r="IK70"/>
-      <c r="IL70"/>
-      <c r="IM70"/>
-      <c r="IN70"/>
-      <c r="IO70"/>
-      <c r="IP70"/>
-      <c r="IQ70"/>
-      <c r="IR70"/>
-      <c r="IS70"/>
-      <c r="IT70"/>
-      <c r="IU70"/>
-      <c r="IV70"/>
-      <c r="IW70"/>
-      <c r="IX70"/>
-      <c r="IY70"/>
-      <c r="IZ70"/>
-      <c r="JA70"/>
-      <c r="JB70"/>
-      <c r="JC70"/>
-      <c r="JD70"/>
-      <c r="JE70"/>
-      <c r="JF70"/>
-      <c r="JG70"/>
-      <c r="JH70"/>
-      <c r="JI70"/>
-      <c r="JJ70"/>
-      <c r="JK70"/>
-      <c r="JL70"/>
-      <c r="JM70"/>
-      <c r="JN70"/>
-      <c r="JO70"/>
-      <c r="JP70"/>
-      <c r="JQ70"/>
-      <c r="JR70"/>
-      <c r="JS70"/>
-      <c r="JT70"/>
-      <c r="JU70"/>
-      <c r="JV70"/>
-      <c r="JW70"/>
-      <c r="JX70"/>
-      <c r="JY70"/>
-      <c r="JZ70"/>
-      <c r="KA70"/>
-      <c r="KB70"/>
-      <c r="KC70"/>
-      <c r="KD70"/>
-      <c r="KE70"/>
-      <c r="KF70"/>
-      <c r="KG70"/>
-      <c r="KH70"/>
-      <c r="KI70"/>
-      <c r="KJ70"/>
-      <c r="KK70"/>
-      <c r="KL70"/>
-      <c r="KM70"/>
-      <c r="KN70"/>
-      <c r="KO70"/>
-      <c r="KP70"/>
-      <c r="KQ70"/>
-      <c r="KR70"/>
-      <c r="KS70"/>
-      <c r="KT70"/>
-      <c r="KU70"/>
-      <c r="KV70"/>
-      <c r="KW70"/>
-      <c r="KX70"/>
-      <c r="KY70"/>
-      <c r="KZ70"/>
-      <c r="LA70"/>
-      <c r="LB70"/>
-      <c r="LC70"/>
-      <c r="LD70"/>
-      <c r="LE70"/>
-      <c r="LF70"/>
-      <c r="LG70"/>
-      <c r="LH70"/>
-      <c r="LI70"/>
-      <c r="LJ70"/>
-      <c r="LK70"/>
-      <c r="LL70"/>
-      <c r="LM70"/>
-      <c r="LN70"/>
-      <c r="LO70"/>
-      <c r="LP70"/>
-      <c r="LQ70"/>
-      <c r="LR70"/>
-      <c r="LS70"/>
-      <c r="LT70"/>
-      <c r="LU70"/>
-      <c r="LV70"/>
-      <c r="LW70"/>
-      <c r="LX70"/>
-      <c r="LY70"/>
-      <c r="LZ70"/>
-      <c r="MA70"/>
-      <c r="MB70"/>
-      <c r="MC70"/>
-      <c r="MD70"/>
-      <c r="ME70"/>
-      <c r="MF70"/>
-      <c r="MG70"/>
-      <c r="MH70"/>
-      <c r="MI70"/>
-      <c r="MJ70"/>
-      <c r="MK70"/>
-      <c r="ML70"/>
-      <c r="MM70"/>
-      <c r="MN70"/>
-      <c r="MO70"/>
-      <c r="MP70"/>
-      <c r="MQ70"/>
-      <c r="MR70"/>
-      <c r="MS70"/>
-      <c r="MT70"/>
-      <c r="MU70"/>
-      <c r="MV70"/>
-      <c r="MW70"/>
-      <c r="MX70"/>
-      <c r="MY70"/>
-      <c r="MZ70"/>
-      <c r="NA70"/>
-      <c r="NB70"/>
-      <c r="NC70"/>
-      <c r="ND70"/>
-      <c r="NE70"/>
-      <c r="NF70"/>
-      <c r="NG70"/>
-      <c r="NH70"/>
-      <c r="NI70"/>
-      <c r="NJ70"/>
-      <c r="NK70"/>
-      <c r="NL70"/>
-      <c r="NM70"/>
-      <c r="NN70"/>
-      <c r="NO70"/>
-      <c r="NP70"/>
-      <c r="NQ70"/>
-      <c r="NR70"/>
-      <c r="NS70"/>
-      <c r="NT70"/>
-      <c r="NU70"/>
-      <c r="NV70"/>
-      <c r="NW70"/>
-      <c r="NX70"/>
-      <c r="NY70"/>
-      <c r="NZ70"/>
-      <c r="OA70"/>
-      <c r="OB70"/>
-      <c r="OC70"/>
-      <c r="OD70"/>
-      <c r="OE70"/>
-      <c r="OF70"/>
-      <c r="OG70"/>
-      <c r="OH70"/>
-      <c r="OI70"/>
-      <c r="OJ70"/>
-      <c r="OK70"/>
-      <c r="OL70"/>
-      <c r="OM70"/>
-      <c r="ON70"/>
-      <c r="OO70"/>
-      <c r="OP70"/>
-      <c r="OQ70"/>
-      <c r="OR70"/>
-      <c r="OS70"/>
-      <c r="OT70"/>
-      <c r="OU70"/>
-      <c r="OV70"/>
-      <c r="OW70"/>
-      <c r="OX70"/>
-      <c r="OY70"/>
-      <c r="OZ70"/>
-      <c r="PA70"/>
-      <c r="PB70"/>
-      <c r="PC70"/>
-      <c r="PD70"/>
-      <c r="PE70"/>
-      <c r="PF70"/>
-      <c r="PG70"/>
-      <c r="PH70"/>
-      <c r="PI70"/>
-      <c r="PJ70"/>
-      <c r="PK70"/>
-      <c r="PL70"/>
-      <c r="PM70"/>
-      <c r="PN70"/>
-      <c r="PO70"/>
-      <c r="PP70"/>
-      <c r="PQ70"/>
-      <c r="PR70"/>
-      <c r="PS70"/>
-      <c r="PT70"/>
-      <c r="PU70"/>
-      <c r="PV70"/>
-      <c r="PW70"/>
-      <c r="PX70"/>
-      <c r="PY70"/>
-      <c r="PZ70"/>
-      <c r="QA70"/>
-      <c r="QB70"/>
-      <c r="QC70"/>
-      <c r="QD70"/>
-      <c r="QE70"/>
-      <c r="QF70"/>
-      <c r="QG70"/>
-      <c r="QH70"/>
-      <c r="QI70"/>
-      <c r="QJ70"/>
-      <c r="QK70"/>
-      <c r="QL70"/>
-      <c r="QM70"/>
-      <c r="QN70"/>
-      <c r="QO70"/>
-      <c r="QP70"/>
-      <c r="QQ70"/>
-      <c r="QR70"/>
-      <c r="QS70"/>
-      <c r="QT70"/>
-      <c r="QU70"/>
-      <c r="QV70"/>
-      <c r="QW70"/>
-      <c r="QX70"/>
-      <c r="QY70"/>
-      <c r="QZ70"/>
-      <c r="RA70"/>
-      <c r="RB70"/>
-      <c r="RC70"/>
-      <c r="RD70"/>
-      <c r="RE70"/>
-      <c r="RF70"/>
-      <c r="RG70"/>
-      <c r="RH70"/>
-      <c r="RI70"/>
-      <c r="RJ70"/>
-      <c r="RK70"/>
-      <c r="RL70"/>
-      <c r="RM70"/>
-      <c r="RN70"/>
-      <c r="RO70"/>
-      <c r="RP70"/>
-      <c r="RQ70"/>
-      <c r="RR70"/>
-      <c r="RS70"/>
-      <c r="RT70"/>
-      <c r="RU70"/>
-      <c r="RV70"/>
-      <c r="RW70"/>
-      <c r="RX70"/>
-      <c r="RY70"/>
-      <c r="RZ70"/>
-      <c r="SA70"/>
-      <c r="SB70"/>
-      <c r="SC70"/>
-      <c r="SD70"/>
-      <c r="SE70"/>
-      <c r="SF70"/>
-      <c r="SG70"/>
-      <c r="SH70"/>
-      <c r="SI70"/>
-      <c r="SJ70"/>
-      <c r="SK70"/>
-      <c r="SL70"/>
-      <c r="SM70"/>
-      <c r="SN70"/>
-      <c r="SO70"/>
-      <c r="SP70"/>
-      <c r="SQ70"/>
-      <c r="SR70"/>
-      <c r="SS70"/>
-      <c r="ST70"/>
-      <c r="SU70"/>
-      <c r="SV70"/>
-      <c r="SW70"/>
-      <c r="SX70"/>
-      <c r="SY70"/>
-      <c r="SZ70"/>
-      <c r="TA70"/>
-      <c r="TB70"/>
-      <c r="TC70"/>
-      <c r="TD70"/>
-      <c r="TE70"/>
-      <c r="TF70"/>
-      <c r="TG70"/>
-      <c r="TH70"/>
-      <c r="TI70"/>
-      <c r="TJ70"/>
-      <c r="TK70"/>
-      <c r="TL70"/>
-      <c r="TM70"/>
-      <c r="TN70"/>
-      <c r="TO70"/>
-      <c r="TP70"/>
-      <c r="TQ70"/>
-      <c r="TR70"/>
-      <c r="TS70"/>
-      <c r="TT70"/>
-      <c r="TU70"/>
-      <c r="TV70"/>
-      <c r="TW70"/>
-      <c r="TX70"/>
-      <c r="TY70"/>
-      <c r="TZ70"/>
-      <c r="UA70"/>
-    </row>
-    <row r="71" spans="1:547" ht="18.600000000000001" thickTop="1">
-      <c r="A71" s="55" t="s">
-        <v>192</v>
-      </c>
-      <c r="B71" s="56"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="57"/>
-    </row>
-    <row r="72" spans="1:547">
-      <c r="A72" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="27"/>
-      <c r="D72" s="42">
+    <row r="90" spans="1:8">
+      <c r="A90" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="40">
+        <v>252</v>
+      </c>
+      <c r="E90" s="29"/>
+      <c r="F90" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G90" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="25"/>
+      <c r="D91" s="40">
+        <v>261</v>
+      </c>
+      <c r="E91" s="29"/>
+      <c r="F91" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" s="53" t="s">
+        <v>203</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="25"/>
+      <c r="D92" s="40">
+        <v>262</v>
+      </c>
+      <c r="E92" s="29"/>
+      <c r="F92" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G72" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H72" s="7"/>
-    </row>
-    <row r="73" spans="1:547">
-      <c r="A73" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="42">
-        <v>201</v>
-      </c>
-      <c r="E73" s="31"/>
-      <c r="F73" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="H73" s="7"/>
-    </row>
-    <row r="74" spans="1:547">
-      <c r="A74" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="27"/>
-      <c r="D74" s="42">
-        <v>202</v>
-      </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:547">
-      <c r="A75" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="42">
-        <v>203</v>
-      </c>
-      <c r="E75" s="31"/>
-      <c r="F75" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:547">
-      <c r="A76" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="27"/>
-      <c r="D76" s="42">
-        <v>204</v>
-      </c>
-      <c r="E76" s="31"/>
-      <c r="F76" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H76" s="7"/>
-    </row>
-    <row r="77" spans="1:547">
-      <c r="A77" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="27"/>
-      <c r="D77" s="42">
-        <v>223</v>
-      </c>
-      <c r="E77" s="31"/>
-      <c r="F77" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G77" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:547">
-      <c r="A78" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="27"/>
-      <c r="D78" s="42">
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="40">
+        <v>263</v>
+      </c>
+      <c r="E93" s="29"/>
+      <c r="F93" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E78" s="31"/>
-      <c r="F78" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H78" s="7"/>
-    </row>
-    <row r="79" spans="1:547">
-      <c r="A79" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="42">
-        <v>242</v>
-      </c>
-      <c r="E79" s="31"/>
-      <c r="F79" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:547">
-      <c r="A80" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B80" s="7"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="42">
-        <v>243</v>
-      </c>
-      <c r="E80" s="31"/>
-      <c r="F80" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="H80" s="7"/>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="42">
-        <v>244</v>
-      </c>
-      <c r="E81" s="31"/>
-      <c r="F81" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="H81" s="7"/>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="27"/>
-      <c r="D82" s="42">
-        <v>245</v>
-      </c>
-      <c r="E82" s="31"/>
-      <c r="F82" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H82" s="7"/>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="49" t="s">
-        <v>210</v>
-      </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="27"/>
-      <c r="D83" s="42">
-        <v>246</v>
-      </c>
-      <c r="E83" s="31"/>
-      <c r="F83" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="H83" s="7"/>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="50" t="s">
-        <v>217</v>
-      </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="27"/>
-      <c r="D84" s="42">
-        <v>247</v>
-      </c>
-      <c r="E84" s="31"/>
-      <c r="F84" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="27"/>
-      <c r="D85" s="42">
-        <v>248</v>
-      </c>
-      <c r="E85" s="31"/>
-      <c r="F85" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="42">
-        <v>249</v>
-      </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="G86" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="49" t="s">
-        <v>207</v>
-      </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="42">
-        <v>250</v>
-      </c>
-      <c r="E87" s="31"/>
-      <c r="F87" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="50" t="s">
-        <v>224</v>
-      </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="42">
-        <v>251</v>
-      </c>
-      <c r="E88" s="31"/>
-      <c r="F88" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>231</v>
-      </c>
-      <c r="H88" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="49" t="s">
+      <c r="G93" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="42">
-        <v>252</v>
-      </c>
-      <c r="E89" s="31"/>
-      <c r="F89" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="G89" s="7" t="s">
-        <v>230</v>
-      </c>
-      <c r="H89" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="50" t="s">
-        <v>188</v>
-      </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="27"/>
-      <c r="D90" s="42">
-        <v>261</v>
-      </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H90" s="9"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="49" t="s">
-        <v>204</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="27"/>
-      <c r="D91" s="42">
-        <v>262</v>
-      </c>
-      <c r="E91" s="31"/>
-      <c r="F91" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="H91" s="9"/>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="50" t="s">
-        <v>221</v>
-      </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="27"/>
-      <c r="D92" s="42">
-        <v>263</v>
-      </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="H92" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="49" t="s">
+      <c r="B94" s="6"/>
+      <c r="C94" s="25"/>
+      <c r="D94" s="40">
+        <v>264</v>
+      </c>
+      <c r="E94" s="29"/>
+      <c r="F94" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="27"/>
-      <c r="D93" s="42">
-        <v>264</v>
-      </c>
-      <c r="E93" s="31"/>
-      <c r="F93" s="7" t="s">
+      <c r="G94" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="G93" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="H93" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="1"/>
-      <c r="H94" s="5"/>
+      <c r="H94" s="8" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="1"/>
-      <c r="H95" s="5"/>
+      <c r="H95" s="4"/>
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="1"/>
-      <c r="H96" s="5"/>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="H96" s="4"/>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="1"/>
-    </row>
-    <row r="98" spans="1:1">
+      <c r="H97" s="4"/>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:8">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:8">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:8">
       <c r="A101" s="1"/>
+    </row>
+    <row r="102" spans="1:8">
+      <c r="A102" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:C17">
@@ -7363,8 +7380,8 @@
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A72:H72"/>
     <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A70:H70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="48" orientation="landscape" r:id="rId1"/>

</xml_diff>